<commit_message>
Punctuation within brackets now does not cause sentence tokenization.
</commit_message>
<xml_diff>
--- a/sentence_pairs_result.xlsx
+++ b/sentence_pairs_result.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="336" uniqueCount="329">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="338" uniqueCount="331">
   <si>
     <t>ja</t>
   </si>
@@ -274,7 +274,10 @@
     <t>FIG. 3は、実施形態の発光部305の構成の一具体例を表す外観図である。</t>
   </si>
   <si>
-    <t>発光部305は、複数の発光素子306-1から発光素子306-nを備える(以下、「発光素子306」という。</t>
+    <t>発光部305は、複数の発光素子306-1から発光素子306-nを備える(以下、「発光素子306」という。)。</t>
+  </si>
+  <si>
+    <t>発光素子306は、発光制御部314からの発光指示に応じて発光する。 強制発光させるデータは、発光指示の一態様である。</t>
   </si>
   <si>
     <t>発光素子306は、画像形成処理中に発光することで、感光体ドラム320に静電潜像を形成させる。</t>
@@ -394,7 +397,7 @@
     <t>制御部310は、画像データの主走査方向の画素数をカウントする変数nに1を設定する(ACT203)。</t>
   </si>
   <si>
-    <t>制御部310は、主走査方向からn番目の画素に対応する発光素子306の累積発光時間の値(以下、「発光時間」という。 )を発光時間記憶部301から取得する(ACT204)。</t>
+    <t>制御部310は、主走査方向からn番目の画素に対応する発光素子306の累積発光時間の値(以下、「発光時間」という。)を発光時間記憶部301から取得する(ACT204)。</t>
   </si>
   <si>
     <t>発光制御部314は、発光時間の値が調整時間の値よりも大きいか否か判定する(ACT205)。</t>
@@ -767,6 +770,9 @@
   </si>
   <si>
     <t>The light emitting unit 305 includes a plurality of light emitting elements 306-1 to 306-n (hereinafter, referred to as "light emitting elements 306").</t>
+  </si>
+  <si>
+    <t>Each of the light emitting elements 306 is connected to the light emission control unitThe light emitting elements 306 emit light in response to a light emission instruction from the light emission control unitData which makes light to be forcibly emitted is an aspect of the light emission instruction.</t>
   </si>
   <si>
     <t>The light emitting elements 306 forms electrostatic latent image in a photosensitive drum 320 by making light to be emitted during image formation processing.</t>
@@ -1358,7 +1364,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:C168"/>
+  <dimension ref="A1:C169"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
@@ -1380,7 +1386,7 @@
         <v>2</v>
       </c>
       <c r="C2" t="s">
-        <v>166</v>
+        <v>167</v>
       </c>
     </row>
     <row r="3" spans="1:3">
@@ -1391,7 +1397,7 @@
         <v>3</v>
       </c>
       <c r="C3" t="s">
-        <v>167</v>
+        <v>168</v>
       </c>
     </row>
     <row r="4" spans="1:3">
@@ -1402,7 +1408,7 @@
         <v>4</v>
       </c>
       <c r="C4" t="s">
-        <v>168</v>
+        <v>169</v>
       </c>
     </row>
     <row r="5" spans="1:3">
@@ -1413,7 +1419,7 @@
         <v>5</v>
       </c>
       <c r="C5" t="s">
-        <v>169</v>
+        <v>170</v>
       </c>
     </row>
     <row r="6" spans="1:3">
@@ -1424,7 +1430,7 @@
         <v>6</v>
       </c>
       <c r="C6" t="s">
-        <v>170</v>
+        <v>171</v>
       </c>
     </row>
     <row r="7" spans="1:3">
@@ -1435,7 +1441,7 @@
         <v>7</v>
       </c>
       <c r="C7" t="s">
-        <v>171</v>
+        <v>172</v>
       </c>
     </row>
     <row r="8" spans="1:3">
@@ -1446,7 +1452,7 @@
         <v>8</v>
       </c>
       <c r="C8" t="s">
-        <v>172</v>
+        <v>173</v>
       </c>
     </row>
     <row r="9" spans="1:3">
@@ -1457,7 +1463,7 @@
         <v>9</v>
       </c>
       <c r="C9" t="s">
-        <v>173</v>
+        <v>174</v>
       </c>
     </row>
     <row r="10" spans="1:3">
@@ -1468,7 +1474,7 @@
         <v>10</v>
       </c>
       <c r="C10" t="s">
-        <v>174</v>
+        <v>175</v>
       </c>
     </row>
     <row r="11" spans="1:3">
@@ -1479,7 +1485,7 @@
         <v>11</v>
       </c>
       <c r="C11" t="s">
-        <v>175</v>
+        <v>176</v>
       </c>
     </row>
     <row r="12" spans="1:3">
@@ -1490,7 +1496,7 @@
         <v>12</v>
       </c>
       <c r="C12" t="s">
-        <v>176</v>
+        <v>177</v>
       </c>
     </row>
     <row r="13" spans="1:3">
@@ -1501,7 +1507,7 @@
         <v>13</v>
       </c>
       <c r="C13" t="s">
-        <v>177</v>
+        <v>178</v>
       </c>
     </row>
     <row r="14" spans="1:3">
@@ -1512,7 +1518,7 @@
         <v>14</v>
       </c>
       <c r="C14" t="s">
-        <v>178</v>
+        <v>179</v>
       </c>
     </row>
     <row r="15" spans="1:3">
@@ -1523,7 +1529,7 @@
         <v>15</v>
       </c>
       <c r="C15" t="s">
-        <v>179</v>
+        <v>180</v>
       </c>
     </row>
     <row r="16" spans="1:3">
@@ -1534,7 +1540,7 @@
         <v>16</v>
       </c>
       <c r="C16" t="s">
-        <v>180</v>
+        <v>181</v>
       </c>
     </row>
     <row r="17" spans="1:3">
@@ -1545,7 +1551,7 @@
         <v>17</v>
       </c>
       <c r="C17" t="s">
-        <v>181</v>
+        <v>182</v>
       </c>
     </row>
     <row r="18" spans="1:3">
@@ -1556,7 +1562,7 @@
         <v>18</v>
       </c>
       <c r="C18" t="s">
-        <v>182</v>
+        <v>183</v>
       </c>
     </row>
     <row r="19" spans="1:3">
@@ -1567,7 +1573,7 @@
         <v>19</v>
       </c>
       <c r="C19" t="s">
-        <v>183</v>
+        <v>184</v>
       </c>
     </row>
     <row r="20" spans="1:3">
@@ -1578,7 +1584,7 @@
         <v>20</v>
       </c>
       <c r="C20" t="s">
-        <v>184</v>
+        <v>185</v>
       </c>
     </row>
     <row r="21" spans="1:3">
@@ -1589,7 +1595,7 @@
         <v>21</v>
       </c>
       <c r="C21" t="s">
-        <v>185</v>
+        <v>186</v>
       </c>
     </row>
     <row r="22" spans="1:3">
@@ -1600,7 +1606,7 @@
         <v>22</v>
       </c>
       <c r="C22" t="s">
-        <v>186</v>
+        <v>187</v>
       </c>
     </row>
     <row r="23" spans="1:3">
@@ -1611,7 +1617,7 @@
         <v>23</v>
       </c>
       <c r="C23" t="s">
-        <v>187</v>
+        <v>188</v>
       </c>
     </row>
     <row r="24" spans="1:3">
@@ -1622,7 +1628,7 @@
         <v>24</v>
       </c>
       <c r="C24" t="s">
-        <v>188</v>
+        <v>189</v>
       </c>
     </row>
     <row r="25" spans="1:3">
@@ -1633,7 +1639,7 @@
         <v>25</v>
       </c>
       <c r="C25" t="s">
-        <v>189</v>
+        <v>190</v>
       </c>
     </row>
     <row r="26" spans="1:3">
@@ -1644,7 +1650,7 @@
         <v>26</v>
       </c>
       <c r="C26" t="s">
-        <v>190</v>
+        <v>191</v>
       </c>
     </row>
     <row r="27" spans="1:3">
@@ -1655,7 +1661,7 @@
         <v>27</v>
       </c>
       <c r="C27" t="s">
-        <v>191</v>
+        <v>192</v>
       </c>
     </row>
     <row r="28" spans="1:3">
@@ -1666,7 +1672,7 @@
         <v>28</v>
       </c>
       <c r="C28" t="s">
-        <v>192</v>
+        <v>193</v>
       </c>
     </row>
     <row r="29" spans="1:3">
@@ -1677,7 +1683,7 @@
         <v>29</v>
       </c>
       <c r="C29" t="s">
-        <v>193</v>
+        <v>194</v>
       </c>
     </row>
     <row r="30" spans="1:3">
@@ -1688,7 +1694,7 @@
         <v>30</v>
       </c>
       <c r="C30" t="s">
-        <v>194</v>
+        <v>195</v>
       </c>
     </row>
     <row r="31" spans="1:3">
@@ -1699,7 +1705,7 @@
         <v>31</v>
       </c>
       <c r="C31" t="s">
-        <v>195</v>
+        <v>196</v>
       </c>
     </row>
     <row r="32" spans="1:3">
@@ -1710,7 +1716,7 @@
         <v>32</v>
       </c>
       <c r="C32" t="s">
-        <v>196</v>
+        <v>197</v>
       </c>
     </row>
     <row r="33" spans="1:3">
@@ -1721,7 +1727,7 @@
         <v>33</v>
       </c>
       <c r="C33" t="s">
-        <v>197</v>
+        <v>198</v>
       </c>
     </row>
     <row r="34" spans="1:3">
@@ -1732,7 +1738,7 @@
         <v>34</v>
       </c>
       <c r="C34" t="s">
-        <v>198</v>
+        <v>199</v>
       </c>
     </row>
     <row r="35" spans="1:3">
@@ -1743,7 +1749,7 @@
         <v>35</v>
       </c>
       <c r="C35" t="s">
-        <v>199</v>
+        <v>200</v>
       </c>
     </row>
     <row r="36" spans="1:3">
@@ -1754,7 +1760,7 @@
         <v>36</v>
       </c>
       <c r="C36" t="s">
-        <v>200</v>
+        <v>201</v>
       </c>
     </row>
     <row r="37" spans="1:3">
@@ -1765,7 +1771,7 @@
         <v>37</v>
       </c>
       <c r="C37" t="s">
-        <v>201</v>
+        <v>202</v>
       </c>
     </row>
     <row r="38" spans="1:3">
@@ -1776,7 +1782,7 @@
         <v>38</v>
       </c>
       <c r="C38" t="s">
-        <v>202</v>
+        <v>203</v>
       </c>
     </row>
     <row r="39" spans="1:3">
@@ -1787,7 +1793,7 @@
         <v>39</v>
       </c>
       <c r="C39" t="s">
-        <v>203</v>
+        <v>204</v>
       </c>
     </row>
     <row r="40" spans="1:3">
@@ -1798,7 +1804,7 @@
         <v>40</v>
       </c>
       <c r="C40" t="s">
-        <v>204</v>
+        <v>205</v>
       </c>
     </row>
     <row r="41" spans="1:3">
@@ -1809,7 +1815,7 @@
         <v>41</v>
       </c>
       <c r="C41" t="s">
-        <v>205</v>
+        <v>206</v>
       </c>
     </row>
     <row r="42" spans="1:3">
@@ -1820,7 +1826,7 @@
         <v>42</v>
       </c>
       <c r="C42" t="s">
-        <v>206</v>
+        <v>207</v>
       </c>
     </row>
     <row r="43" spans="1:3">
@@ -1831,7 +1837,7 @@
         <v>43</v>
       </c>
       <c r="C43" t="s">
-        <v>207</v>
+        <v>208</v>
       </c>
     </row>
     <row r="44" spans="1:3">
@@ -1842,7 +1848,7 @@
         <v>44</v>
       </c>
       <c r="C44" t="s">
-        <v>208</v>
+        <v>209</v>
       </c>
     </row>
     <row r="45" spans="1:3">
@@ -1853,7 +1859,7 @@
         <v>45</v>
       </c>
       <c r="C45" t="s">
-        <v>209</v>
+        <v>210</v>
       </c>
     </row>
     <row r="46" spans="1:3">
@@ -1864,7 +1870,7 @@
         <v>46</v>
       </c>
       <c r="C46" t="s">
-        <v>210</v>
+        <v>211</v>
       </c>
     </row>
     <row r="47" spans="1:3">
@@ -1875,7 +1881,7 @@
         <v>47</v>
       </c>
       <c r="C47" t="s">
-        <v>211</v>
+        <v>212</v>
       </c>
     </row>
     <row r="48" spans="1:3">
@@ -1886,7 +1892,7 @@
         <v>48</v>
       </c>
       <c r="C48" t="s">
-        <v>212</v>
+        <v>213</v>
       </c>
     </row>
     <row r="49" spans="1:3">
@@ -1897,7 +1903,7 @@
         <v>49</v>
       </c>
       <c r="C49" t="s">
-        <v>213</v>
+        <v>214</v>
       </c>
     </row>
     <row r="50" spans="1:3">
@@ -1908,7 +1914,7 @@
         <v>50</v>
       </c>
       <c r="C50" t="s">
-        <v>214</v>
+        <v>215</v>
       </c>
     </row>
     <row r="51" spans="1:3">
@@ -1919,7 +1925,7 @@
         <v>51</v>
       </c>
       <c r="C51" t="s">
-        <v>215</v>
+        <v>216</v>
       </c>
     </row>
     <row r="52" spans="1:3">
@@ -1930,7 +1936,7 @@
         <v>52</v>
       </c>
       <c r="C52" t="s">
-        <v>216</v>
+        <v>217</v>
       </c>
     </row>
     <row r="53" spans="1:3">
@@ -1941,7 +1947,7 @@
         <v>53</v>
       </c>
       <c r="C53" t="s">
-        <v>217</v>
+        <v>218</v>
       </c>
     </row>
     <row r="54" spans="1:3">
@@ -1952,7 +1958,7 @@
         <v>54</v>
       </c>
       <c r="C54" t="s">
-        <v>218</v>
+        <v>219</v>
       </c>
     </row>
     <row r="55" spans="1:3">
@@ -1963,7 +1969,7 @@
         <v>55</v>
       </c>
       <c r="C55" t="s">
-        <v>219</v>
+        <v>220</v>
       </c>
     </row>
     <row r="56" spans="1:3">
@@ -1974,7 +1980,7 @@
         <v>56</v>
       </c>
       <c r="C56" t="s">
-        <v>220</v>
+        <v>221</v>
       </c>
     </row>
     <row r="57" spans="1:3">
@@ -1985,7 +1991,7 @@
         <v>57</v>
       </c>
       <c r="C57" t="s">
-        <v>221</v>
+        <v>222</v>
       </c>
     </row>
     <row r="58" spans="1:3">
@@ -1996,7 +2002,7 @@
         <v>58</v>
       </c>
       <c r="C58" t="s">
-        <v>222</v>
+        <v>223</v>
       </c>
     </row>
     <row r="59" spans="1:3">
@@ -2007,7 +2013,7 @@
         <v>59</v>
       </c>
       <c r="C59" t="s">
-        <v>223</v>
+        <v>224</v>
       </c>
     </row>
     <row r="60" spans="1:3">
@@ -2018,7 +2024,7 @@
         <v>60</v>
       </c>
       <c r="C60" t="s">
-        <v>224</v>
+        <v>225</v>
       </c>
     </row>
     <row r="61" spans="1:3">
@@ -2029,7 +2035,7 @@
         <v>61</v>
       </c>
       <c r="C61" t="s">
-        <v>225</v>
+        <v>226</v>
       </c>
     </row>
     <row r="62" spans="1:3">
@@ -2040,7 +2046,7 @@
         <v>62</v>
       </c>
       <c r="C62" t="s">
-        <v>226</v>
+        <v>227</v>
       </c>
     </row>
     <row r="63" spans="1:3">
@@ -2051,7 +2057,7 @@
         <v>63</v>
       </c>
       <c r="C63" t="s">
-        <v>227</v>
+        <v>228</v>
       </c>
     </row>
     <row r="64" spans="1:3">
@@ -2062,7 +2068,7 @@
         <v>64</v>
       </c>
       <c r="C64" t="s">
-        <v>228</v>
+        <v>229</v>
       </c>
     </row>
     <row r="65" spans="1:3">
@@ -2073,7 +2079,7 @@
         <v>65</v>
       </c>
       <c r="C65" t="s">
-        <v>229</v>
+        <v>230</v>
       </c>
     </row>
     <row r="66" spans="1:3">
@@ -2084,7 +2090,7 @@
         <v>66</v>
       </c>
       <c r="C66" t="s">
-        <v>230</v>
+        <v>231</v>
       </c>
     </row>
     <row r="67" spans="1:3">
@@ -2095,7 +2101,7 @@
         <v>67</v>
       </c>
       <c r="C67" t="s">
-        <v>231</v>
+        <v>232</v>
       </c>
     </row>
     <row r="68" spans="1:3">
@@ -2106,7 +2112,7 @@
         <v>68</v>
       </c>
       <c r="C68" t="s">
-        <v>232</v>
+        <v>233</v>
       </c>
     </row>
     <row r="69" spans="1:3">
@@ -2117,7 +2123,7 @@
         <v>69</v>
       </c>
       <c r="C69" t="s">
-        <v>233</v>
+        <v>234</v>
       </c>
     </row>
     <row r="70" spans="1:3">
@@ -2128,7 +2134,7 @@
         <v>70</v>
       </c>
       <c r="C70" t="s">
-        <v>234</v>
+        <v>235</v>
       </c>
     </row>
     <row r="71" spans="1:3">
@@ -2139,7 +2145,7 @@
         <v>71</v>
       </c>
       <c r="C71" t="s">
-        <v>235</v>
+        <v>236</v>
       </c>
     </row>
     <row r="72" spans="1:3">
@@ -2150,7 +2156,7 @@
         <v>72</v>
       </c>
       <c r="C72" t="s">
-        <v>236</v>
+        <v>237</v>
       </c>
     </row>
     <row r="73" spans="1:3">
@@ -2161,7 +2167,7 @@
         <v>73</v>
       </c>
       <c r="C73" t="s">
-        <v>237</v>
+        <v>238</v>
       </c>
     </row>
     <row r="74" spans="1:3">
@@ -2172,7 +2178,7 @@
         <v>74</v>
       </c>
       <c r="C74" t="s">
-        <v>238</v>
+        <v>239</v>
       </c>
     </row>
     <row r="75" spans="1:3">
@@ -2183,7 +2189,7 @@
         <v>75</v>
       </c>
       <c r="C75" t="s">
-        <v>239</v>
+        <v>240</v>
       </c>
     </row>
     <row r="76" spans="1:3">
@@ -2194,7 +2200,7 @@
         <v>76</v>
       </c>
       <c r="C76" t="s">
-        <v>240</v>
+        <v>241</v>
       </c>
     </row>
     <row r="77" spans="1:3">
@@ -2205,7 +2211,7 @@
         <v>77</v>
       </c>
       <c r="C77" t="s">
-        <v>241</v>
+        <v>242</v>
       </c>
     </row>
     <row r="78" spans="1:3">
@@ -2216,7 +2222,7 @@
         <v>78</v>
       </c>
       <c r="C78" t="s">
-        <v>242</v>
+        <v>243</v>
       </c>
     </row>
     <row r="79" spans="1:3">
@@ -2227,7 +2233,7 @@
         <v>79</v>
       </c>
       <c r="C79" t="s">
-        <v>243</v>
+        <v>244</v>
       </c>
     </row>
     <row r="80" spans="1:3">
@@ -2238,7 +2244,7 @@
         <v>80</v>
       </c>
       <c r="C80" t="s">
-        <v>244</v>
+        <v>245</v>
       </c>
     </row>
     <row r="81" spans="1:3">
@@ -2249,7 +2255,7 @@
         <v>81</v>
       </c>
       <c r="C81" t="s">
-        <v>245</v>
+        <v>246</v>
       </c>
     </row>
     <row r="82" spans="1:3">
@@ -2260,7 +2266,7 @@
         <v>82</v>
       </c>
       <c r="C82" t="s">
-        <v>246</v>
+        <v>247</v>
       </c>
     </row>
     <row r="83" spans="1:3">
@@ -2271,7 +2277,7 @@
         <v>83</v>
       </c>
       <c r="C83" t="s">
-        <v>247</v>
+        <v>248</v>
       </c>
     </row>
     <row r="84" spans="1:3">
@@ -2282,7 +2288,7 @@
         <v>84</v>
       </c>
       <c r="C84" t="s">
-        <v>248</v>
+        <v>249</v>
       </c>
     </row>
     <row r="85" spans="1:3">
@@ -2293,7 +2299,7 @@
         <v>85</v>
       </c>
       <c r="C85" t="s">
-        <v>249</v>
+        <v>250</v>
       </c>
     </row>
     <row r="86" spans="1:3">
@@ -2304,7 +2310,7 @@
         <v>86</v>
       </c>
       <c r="C86" t="s">
-        <v>250</v>
+        <v>251</v>
       </c>
     </row>
     <row r="87" spans="1:3">
@@ -2315,7 +2321,7 @@
         <v>87</v>
       </c>
       <c r="C87" t="s">
-        <v>251</v>
+        <v>252</v>
       </c>
     </row>
     <row r="88" spans="1:3">
@@ -2326,7 +2332,7 @@
         <v>88</v>
       </c>
       <c r="C88" t="s">
-        <v>252</v>
+        <v>253</v>
       </c>
     </row>
     <row r="89" spans="1:3">
@@ -2337,7 +2343,7 @@
         <v>89</v>
       </c>
       <c r="C89" t="s">
-        <v>253</v>
+        <v>254</v>
       </c>
     </row>
     <row r="90" spans="1:3">
@@ -2348,7 +2354,7 @@
         <v>90</v>
       </c>
       <c r="C90" t="s">
-        <v>254</v>
+        <v>255</v>
       </c>
     </row>
     <row r="91" spans="1:3">
@@ -2359,7 +2365,7 @@
         <v>91</v>
       </c>
       <c r="C91" t="s">
-        <v>255</v>
+        <v>256</v>
       </c>
     </row>
     <row r="92" spans="1:3">
@@ -2370,7 +2376,7 @@
         <v>92</v>
       </c>
       <c r="C92" t="s">
-        <v>256</v>
+        <v>257</v>
       </c>
     </row>
     <row r="93" spans="1:3">
@@ -2381,7 +2387,7 @@
         <v>93</v>
       </c>
       <c r="C93" t="s">
-        <v>257</v>
+        <v>258</v>
       </c>
     </row>
     <row r="94" spans="1:3">
@@ -2392,7 +2398,7 @@
         <v>94</v>
       </c>
       <c r="C94" t="s">
-        <v>258</v>
+        <v>259</v>
       </c>
     </row>
     <row r="95" spans="1:3">
@@ -2403,7 +2409,7 @@
         <v>95</v>
       </c>
       <c r="C95" t="s">
-        <v>259</v>
+        <v>260</v>
       </c>
     </row>
     <row r="96" spans="1:3">
@@ -2414,7 +2420,7 @@
         <v>96</v>
       </c>
       <c r="C96" t="s">
-        <v>260</v>
+        <v>261</v>
       </c>
     </row>
     <row r="97" spans="1:3">
@@ -2425,7 +2431,7 @@
         <v>97</v>
       </c>
       <c r="C97" t="s">
-        <v>261</v>
+        <v>262</v>
       </c>
     </row>
     <row r="98" spans="1:3">
@@ -2436,7 +2442,7 @@
         <v>98</v>
       </c>
       <c r="C98" t="s">
-        <v>262</v>
+        <v>263</v>
       </c>
     </row>
     <row r="99" spans="1:3">
@@ -2447,7 +2453,7 @@
         <v>99</v>
       </c>
       <c r="C99" t="s">
-        <v>263</v>
+        <v>264</v>
       </c>
     </row>
     <row r="100" spans="1:3">
@@ -2458,7 +2464,7 @@
         <v>100</v>
       </c>
       <c r="C100" t="s">
-        <v>264</v>
+        <v>265</v>
       </c>
     </row>
     <row r="101" spans="1:3">
@@ -2469,7 +2475,7 @@
         <v>101</v>
       </c>
       <c r="C101" t="s">
-        <v>265</v>
+        <v>266</v>
       </c>
     </row>
     <row r="102" spans="1:3">
@@ -2480,7 +2486,7 @@
         <v>102</v>
       </c>
       <c r="C102" t="s">
-        <v>266</v>
+        <v>267</v>
       </c>
     </row>
     <row r="103" spans="1:3">
@@ -2491,7 +2497,7 @@
         <v>103</v>
       </c>
       <c r="C103" t="s">
-        <v>267</v>
+        <v>268</v>
       </c>
     </row>
     <row r="104" spans="1:3">
@@ -2502,7 +2508,7 @@
         <v>104</v>
       </c>
       <c r="C104" t="s">
-        <v>268</v>
+        <v>269</v>
       </c>
     </row>
     <row r="105" spans="1:3">
@@ -2513,7 +2519,7 @@
         <v>105</v>
       </c>
       <c r="C105" t="s">
-        <v>269</v>
+        <v>270</v>
       </c>
     </row>
     <row r="106" spans="1:3">
@@ -2524,7 +2530,7 @@
         <v>106</v>
       </c>
       <c r="C106" t="s">
-        <v>270</v>
+        <v>271</v>
       </c>
     </row>
     <row r="107" spans="1:3">
@@ -2535,7 +2541,7 @@
         <v>107</v>
       </c>
       <c r="C107" t="s">
-        <v>271</v>
+        <v>272</v>
       </c>
     </row>
     <row r="108" spans="1:3">
@@ -2546,7 +2552,7 @@
         <v>108</v>
       </c>
       <c r="C108" t="s">
-        <v>272</v>
+        <v>273</v>
       </c>
     </row>
     <row r="109" spans="1:3">
@@ -2557,7 +2563,7 @@
         <v>109</v>
       </c>
       <c r="C109" t="s">
-        <v>273</v>
+        <v>274</v>
       </c>
     </row>
     <row r="110" spans="1:3">
@@ -2568,7 +2574,7 @@
         <v>110</v>
       </c>
       <c r="C110" t="s">
-        <v>274</v>
+        <v>275</v>
       </c>
     </row>
     <row r="111" spans="1:3">
@@ -2579,7 +2585,7 @@
         <v>111</v>
       </c>
       <c r="C111" t="s">
-        <v>275</v>
+        <v>276</v>
       </c>
     </row>
     <row r="112" spans="1:3">
@@ -2590,7 +2596,7 @@
         <v>112</v>
       </c>
       <c r="C112" t="s">
-        <v>276</v>
+        <v>277</v>
       </c>
     </row>
     <row r="113" spans="1:3">
@@ -2601,7 +2607,7 @@
         <v>113</v>
       </c>
       <c r="C113" t="s">
-        <v>277</v>
+        <v>278</v>
       </c>
     </row>
     <row r="114" spans="1:3">
@@ -2612,7 +2618,7 @@
         <v>114</v>
       </c>
       <c r="C114" t="s">
-        <v>278</v>
+        <v>279</v>
       </c>
     </row>
     <row r="115" spans="1:3">
@@ -2623,7 +2629,7 @@
         <v>115</v>
       </c>
       <c r="C115" t="s">
-        <v>279</v>
+        <v>280</v>
       </c>
     </row>
     <row r="116" spans="1:3">
@@ -2634,7 +2640,7 @@
         <v>116</v>
       </c>
       <c r="C116" t="s">
-        <v>280</v>
+        <v>281</v>
       </c>
     </row>
     <row r="117" spans="1:3">
@@ -2645,7 +2651,7 @@
         <v>117</v>
       </c>
       <c r="C117" t="s">
-        <v>281</v>
+        <v>282</v>
       </c>
     </row>
     <row r="118" spans="1:3">
@@ -2656,7 +2662,7 @@
         <v>118</v>
       </c>
       <c r="C118" t="s">
-        <v>282</v>
+        <v>283</v>
       </c>
     </row>
     <row r="119" spans="1:3">
@@ -2667,7 +2673,7 @@
         <v>119</v>
       </c>
       <c r="C119" t="s">
-        <v>283</v>
+        <v>284</v>
       </c>
     </row>
     <row r="120" spans="1:3">
@@ -2678,7 +2684,7 @@
         <v>120</v>
       </c>
       <c r="C120" t="s">
-        <v>284</v>
+        <v>285</v>
       </c>
     </row>
     <row r="121" spans="1:3">
@@ -2689,7 +2695,7 @@
         <v>121</v>
       </c>
       <c r="C121" t="s">
-        <v>285</v>
+        <v>286</v>
       </c>
     </row>
     <row r="122" spans="1:3">
@@ -2700,7 +2706,7 @@
         <v>122</v>
       </c>
       <c r="C122" t="s">
-        <v>286</v>
+        <v>287</v>
       </c>
     </row>
     <row r="123" spans="1:3">
@@ -2711,7 +2717,7 @@
         <v>123</v>
       </c>
       <c r="C123" t="s">
-        <v>287</v>
+        <v>288</v>
       </c>
     </row>
     <row r="124" spans="1:3">
@@ -2722,7 +2728,7 @@
         <v>124</v>
       </c>
       <c r="C124" t="s">
-        <v>288</v>
+        <v>289</v>
       </c>
     </row>
     <row r="125" spans="1:3">
@@ -2733,7 +2739,7 @@
         <v>125</v>
       </c>
       <c r="C125" t="s">
-        <v>289</v>
+        <v>290</v>
       </c>
     </row>
     <row r="126" spans="1:3">
@@ -2744,7 +2750,7 @@
         <v>126</v>
       </c>
       <c r="C126" t="s">
-        <v>290</v>
+        <v>291</v>
       </c>
     </row>
     <row r="127" spans="1:3">
@@ -2755,7 +2761,7 @@
         <v>127</v>
       </c>
       <c r="C127" t="s">
-        <v>291</v>
+        <v>292</v>
       </c>
     </row>
     <row r="128" spans="1:3">
@@ -2766,7 +2772,7 @@
         <v>128</v>
       </c>
       <c r="C128" t="s">
-        <v>292</v>
+        <v>293</v>
       </c>
     </row>
     <row r="129" spans="1:3">
@@ -2777,7 +2783,7 @@
         <v>129</v>
       </c>
       <c r="C129" t="s">
-        <v>293</v>
+        <v>294</v>
       </c>
     </row>
     <row r="130" spans="1:3">
@@ -2788,7 +2794,7 @@
         <v>130</v>
       </c>
       <c r="C130" t="s">
-        <v>294</v>
+        <v>295</v>
       </c>
     </row>
     <row r="131" spans="1:3">
@@ -2799,7 +2805,7 @@
         <v>131</v>
       </c>
       <c r="C131" t="s">
-        <v>295</v>
+        <v>296</v>
       </c>
     </row>
     <row r="132" spans="1:3">
@@ -2810,7 +2816,7 @@
         <v>132</v>
       </c>
       <c r="C132" t="s">
-        <v>296</v>
+        <v>297</v>
       </c>
     </row>
     <row r="133" spans="1:3">
@@ -2821,7 +2827,7 @@
         <v>133</v>
       </c>
       <c r="C133" t="s">
-        <v>297</v>
+        <v>298</v>
       </c>
     </row>
     <row r="134" spans="1:3">
@@ -2832,7 +2838,7 @@
         <v>134</v>
       </c>
       <c r="C134" t="s">
-        <v>298</v>
+        <v>299</v>
       </c>
     </row>
     <row r="135" spans="1:3">
@@ -2843,7 +2849,7 @@
         <v>135</v>
       </c>
       <c r="C135" t="s">
-        <v>299</v>
+        <v>300</v>
       </c>
     </row>
     <row r="136" spans="1:3">
@@ -2854,7 +2860,7 @@
         <v>136</v>
       </c>
       <c r="C136" t="s">
-        <v>300</v>
+        <v>301</v>
       </c>
     </row>
     <row r="137" spans="1:3">
@@ -2865,7 +2871,7 @@
         <v>137</v>
       </c>
       <c r="C137" t="s">
-        <v>301</v>
+        <v>302</v>
       </c>
     </row>
     <row r="138" spans="1:3">
@@ -2876,7 +2882,7 @@
         <v>138</v>
       </c>
       <c r="C138" t="s">
-        <v>302</v>
+        <v>303</v>
       </c>
     </row>
     <row r="139" spans="1:3">
@@ -2887,7 +2893,7 @@
         <v>139</v>
       </c>
       <c r="C139" t="s">
-        <v>303</v>
+        <v>304</v>
       </c>
     </row>
     <row r="140" spans="1:3">
@@ -2898,7 +2904,7 @@
         <v>140</v>
       </c>
       <c r="C140" t="s">
-        <v>304</v>
+        <v>305</v>
       </c>
     </row>
     <row r="141" spans="1:3">
@@ -2909,7 +2915,7 @@
         <v>141</v>
       </c>
       <c r="C141" t="s">
-        <v>305</v>
+        <v>306</v>
       </c>
     </row>
     <row r="142" spans="1:3">
@@ -2920,7 +2926,7 @@
         <v>142</v>
       </c>
       <c r="C142" t="s">
-        <v>306</v>
+        <v>307</v>
       </c>
     </row>
     <row r="143" spans="1:3">
@@ -2931,7 +2937,7 @@
         <v>143</v>
       </c>
       <c r="C143" t="s">
-        <v>307</v>
+        <v>308</v>
       </c>
     </row>
     <row r="144" spans="1:3">
@@ -2942,7 +2948,7 @@
         <v>144</v>
       </c>
       <c r="C144" t="s">
-        <v>308</v>
+        <v>309</v>
       </c>
     </row>
     <row r="145" spans="1:3">
@@ -2953,7 +2959,7 @@
         <v>145</v>
       </c>
       <c r="C145" t="s">
-        <v>309</v>
+        <v>310</v>
       </c>
     </row>
     <row r="146" spans="1:3">
@@ -2964,7 +2970,7 @@
         <v>146</v>
       </c>
       <c r="C146" t="s">
-        <v>310</v>
+        <v>311</v>
       </c>
     </row>
     <row r="147" spans="1:3">
@@ -2975,7 +2981,7 @@
         <v>147</v>
       </c>
       <c r="C147" t="s">
-        <v>311</v>
+        <v>312</v>
       </c>
     </row>
     <row r="148" spans="1:3">
@@ -2986,7 +2992,7 @@
         <v>148</v>
       </c>
       <c r="C148" t="s">
-        <v>312</v>
+        <v>313</v>
       </c>
     </row>
     <row r="149" spans="1:3">
@@ -2997,7 +3003,7 @@
         <v>149</v>
       </c>
       <c r="C149" t="s">
-        <v>313</v>
+        <v>314</v>
       </c>
     </row>
     <row r="150" spans="1:3">
@@ -3008,7 +3014,7 @@
         <v>150</v>
       </c>
       <c r="C150" t="s">
-        <v>314</v>
+        <v>315</v>
       </c>
     </row>
     <row r="151" spans="1:3">
@@ -3019,7 +3025,7 @@
         <v>151</v>
       </c>
       <c r="C151" t="s">
-        <v>315</v>
+        <v>316</v>
       </c>
     </row>
     <row r="152" spans="1:3">
@@ -3030,7 +3036,7 @@
         <v>152</v>
       </c>
       <c r="C152" t="s">
-        <v>316</v>
+        <v>317</v>
       </c>
     </row>
     <row r="153" spans="1:3">
@@ -3041,7 +3047,7 @@
         <v>153</v>
       </c>
       <c r="C153" t="s">
-        <v>317</v>
+        <v>318</v>
       </c>
     </row>
     <row r="154" spans="1:3">
@@ -3052,7 +3058,7 @@
         <v>154</v>
       </c>
       <c r="C154" t="s">
-        <v>318</v>
+        <v>319</v>
       </c>
     </row>
     <row r="155" spans="1:3">
@@ -3063,7 +3069,7 @@
         <v>155</v>
       </c>
       <c r="C155" t="s">
-        <v>319</v>
+        <v>320</v>
       </c>
     </row>
     <row r="156" spans="1:3">
@@ -3074,7 +3080,7 @@
         <v>156</v>
       </c>
       <c r="C156" t="s">
-        <v>320</v>
+        <v>321</v>
       </c>
     </row>
     <row r="157" spans="1:3">
@@ -3082,10 +3088,10 @@
         <v>156</v>
       </c>
       <c r="B157" t="s">
-        <v>150</v>
+        <v>157</v>
       </c>
       <c r="C157" t="s">
-        <v>314</v>
+        <v>322</v>
       </c>
     </row>
     <row r="158" spans="1:3">
@@ -3093,10 +3099,10 @@
         <v>157</v>
       </c>
       <c r="B158" t="s">
-        <v>157</v>
+        <v>151</v>
       </c>
       <c r="C158" t="s">
-        <v>321</v>
+        <v>316</v>
       </c>
     </row>
     <row r="159" spans="1:3">
@@ -3107,7 +3113,7 @@
         <v>158</v>
       </c>
       <c r="C159" t="s">
-        <v>322</v>
+        <v>323</v>
       </c>
     </row>
     <row r="160" spans="1:3">
@@ -3118,7 +3124,7 @@
         <v>159</v>
       </c>
       <c r="C160" t="s">
-        <v>323</v>
+        <v>324</v>
       </c>
     </row>
     <row r="161" spans="1:3">
@@ -3129,7 +3135,7 @@
         <v>160</v>
       </c>
       <c r="C161" t="s">
-        <v>324</v>
+        <v>325</v>
       </c>
     </row>
     <row r="162" spans="1:3">
@@ -3140,7 +3146,7 @@
         <v>161</v>
       </c>
       <c r="C162" t="s">
-        <v>325</v>
+        <v>326</v>
       </c>
     </row>
     <row r="163" spans="1:3">
@@ -3151,7 +3157,7 @@
         <v>162</v>
       </c>
       <c r="C163" t="s">
-        <v>326</v>
+        <v>327</v>
       </c>
     </row>
     <row r="164" spans="1:3">
@@ -3162,7 +3168,7 @@
         <v>163</v>
       </c>
       <c r="C164" t="s">
-        <v>327</v>
+        <v>328</v>
       </c>
     </row>
     <row r="165" spans="1:3">
@@ -3173,7 +3179,7 @@
         <v>164</v>
       </c>
       <c r="C165" t="s">
-        <v>328</v>
+        <v>329</v>
       </c>
     </row>
     <row r="166" spans="1:3">
@@ -3181,10 +3187,10 @@
         <v>165</v>
       </c>
       <c r="B166" t="s">
-        <v>21</v>
+        <v>165</v>
       </c>
       <c r="C166" t="s">
-        <v>185</v>
+        <v>330</v>
       </c>
     </row>
     <row r="167" spans="1:3">
@@ -3192,7 +3198,7 @@
         <v>166</v>
       </c>
       <c r="B167" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="C167" t="s">
         <v>186</v>
@@ -3203,10 +3209,21 @@
         <v>167</v>
       </c>
       <c r="B168" t="s">
-        <v>165</v>
+        <v>22</v>
       </c>
       <c r="C168" t="s">
         <v>187</v>
+      </c>
+    </row>
+    <row r="169" spans="1:3">
+      <c r="A169" s="1">
+        <v>168</v>
+      </c>
+      <c r="B169" t="s">
+        <v>166</v>
+      </c>
+      <c r="C169" t="s">
+        <v>188</v>
       </c>
     </row>
   </sheetData>

</xml_diff>